<commit_message>
TC for opening new tab. done
</commit_message>
<xml_diff>
--- a/TestCases/TestCases for chrome_newtab.xlsx
+++ b/TestCases/TestCases for chrome_newtab.xlsx
@@ -18,14 +18,99 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+  <si>
+    <t>Google Chrome new tab</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Actual result</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Opening new tab</t>
+  </si>
+  <si>
+    <t>Opening new tab on click on the "new tab" button</t>
+  </si>
+  <si>
+    <t>1. Launch the GoogleChrome browser. 
+2. Click on the "new tab" button</t>
+  </si>
+  <si>
+    <t>Preconditions</t>
+  </si>
+  <si>
+    <t>Latest stable version of GoogleChrome installed</t>
+  </si>
+  <si>
+    <t>New tab is opened</t>
+  </si>
+  <si>
+    <t>GoogleChrome 96.0.4664.110</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>Opening new tab via address bar</t>
+  </si>
+  <si>
+    <t>Opening new tab by address "chrome://newtab" in address bar</t>
+  </si>
+  <si>
+    <t>1. Launch the GoogleChrome browser. 
+2. Open any site (to have posibility to see result)
+3. Type on address bar "chrome://newtab"
+4. Press "Enter"</t>
+  </si>
+  <si>
+    <t>Opening new tab with hotkey</t>
+  </si>
+  <si>
+    <t>Opening new tab with hotkey "Ctrl+N"</t>
+  </si>
+  <si>
+    <t>1. Launch the GoogleChrome browser. 
+2. Press Ctrl+N</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -37,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -45,15 +130,308 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,9 +447,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -109,12 +487,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +527,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -181,7 +559,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -331,12 +709,528 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>2</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>3</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="19"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="C23:M23"/>
+    <mergeCell ref="C24:M24"/>
+    <mergeCell ref="C25:M25"/>
+    <mergeCell ref="C14:M14"/>
+    <mergeCell ref="C15:M15"/>
+    <mergeCell ref="C16:M16"/>
+    <mergeCell ref="C17:M17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="C18:M18"/>
+    <mergeCell ref="C19:M19"/>
+    <mergeCell ref="C20:M20"/>
+    <mergeCell ref="C21:M21"/>
+    <mergeCell ref="C22:M22"/>
+    <mergeCell ref="C8:M8"/>
+    <mergeCell ref="C9:M9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="C10:M10"/>
+    <mergeCell ref="C11:M11"/>
+    <mergeCell ref="C12:M12"/>
+    <mergeCell ref="C13:M13"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some fixes. Incorrect hotkey. CTRL+T insteed CTRL+N
</commit_message>
<xml_diff>
--- a/TestCases/TestCases for chrome_newtab.xlsx
+++ b/TestCases/TestCases for chrome_newtab.xlsx
@@ -85,11 +85,11 @@
     <t>Opening new tab with hotkey</t>
   </si>
   <si>
-    <t>Opening new tab with hotkey "Ctrl+N"</t>
+    <t>Opening new tab with hotkey "Ctrl+T"</t>
   </si>
   <si>
     <t>1. Launch the GoogleChrome browser. 
-2. Press Ctrl+N</t>
+2. Press Ctrl+T</t>
   </si>
 </sst>
 </file>
@@ -375,49 +375,49 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -426,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -712,7 +712,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,84 +721,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="17" t="s">
@@ -816,143 +816,143 @@
       <c r="M5" s="19"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="4"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -970,143 +970,143 @@
       <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="10">
         <v>3</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="4"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="15" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="17" t="s">
@@ -1124,83 +1124,104 @@
       <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="16" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="C10:M10"/>
+    <mergeCell ref="C11:M11"/>
+    <mergeCell ref="C12:M12"/>
+    <mergeCell ref="C13:M13"/>
+    <mergeCell ref="C8:M8"/>
+    <mergeCell ref="C9:M9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="C5:M5"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="C18:M18"/>
+    <mergeCell ref="C19:M19"/>
+    <mergeCell ref="C20:M20"/>
+    <mergeCell ref="C21:M21"/>
+    <mergeCell ref="C22:M22"/>
     <mergeCell ref="C23:M23"/>
     <mergeCell ref="C24:M24"/>
     <mergeCell ref="C25:M25"/>
@@ -1208,27 +1229,6 @@
     <mergeCell ref="C15:M15"/>
     <mergeCell ref="C16:M16"/>
     <mergeCell ref="C17:M17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="C18:M18"/>
-    <mergeCell ref="C19:M19"/>
-    <mergeCell ref="C20:M20"/>
-    <mergeCell ref="C21:M21"/>
-    <mergeCell ref="C22:M22"/>
-    <mergeCell ref="C8:M8"/>
-    <mergeCell ref="C9:M9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="C10:M10"/>
-    <mergeCell ref="C11:M11"/>
-    <mergeCell ref="C12:M12"/>
-    <mergeCell ref="C13:M13"/>
-    <mergeCell ref="C2:M2"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="C5:M5"/>
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="C7:M7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>